<commit_message>
Updates to ROIC calcs
</commit_message>
<xml_diff>
--- a/Files/Statement Lines Lookup.xlsx
+++ b/Files/Statement Lines Lookup.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jburkhow\Google Drive\Documents\GitHub\rule_one\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C0830858-D394-41BB-8D20-31FAE1B599D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CEF33CFB-5104-4D21-9635-E1E9483C5AE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7369A19D-FF00-46E8-8440-BD705B9140C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="473" xr2:uid="{7369A19D-FF00-46E8-8440-BD705B9140C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Unmapped Lines" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unmapped Lines'!$A$1:$C$58</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="251">
   <si>
     <t>Accounts Payable</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Accounts Receivable</t>
   </si>
   <si>
-    <t>Accrued expenses</t>
-  </si>
-  <si>
     <t>Cash</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Inventory</t>
   </si>
   <si>
-    <t>Long term debt</t>
-  </si>
-  <si>
     <t>Noncontrolling Interests</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Salaries and Benefits</t>
   </si>
   <si>
-    <t>Tax rate assumption</t>
-  </si>
-  <si>
     <t>Taxes</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>GeneralAndAdministrativeExpense</t>
   </si>
   <si>
-    <t>ResearchAndDevelopmentExpense</t>
-  </si>
-  <si>
     <t>OperatingIncomeLoss</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>IncomeTaxExpenseBenefit</t>
   </si>
   <si>
-    <t>NetIncomeLossAttributableToNoncontrollingInterest</t>
-  </si>
-  <si>
     <t>EarningsPerShareBasic</t>
   </si>
   <si>
@@ -335,9 +320,6 @@
     <t>OtherAssetsNoncurrent</t>
   </si>
   <si>
-    <t>OtherLiabilitiesCurrent</t>
-  </si>
-  <si>
     <t>PayableForRepurchaseOfCommonStocks</t>
   </si>
   <si>
@@ -729,6 +711,78 @@
   </si>
   <si>
     <t>Current Liabilities</t>
+  </si>
+  <si>
+    <t>Revenues</t>
+  </si>
+  <si>
+    <t>Noncurrent Liabilities</t>
+  </si>
+  <si>
+    <t>OtherLiabilitiesNoncurrent</t>
+  </si>
+  <si>
+    <t>DepreciationAndAmortization</t>
+  </si>
+  <si>
+    <t>Book Value of Debt</t>
+  </si>
+  <si>
+    <t>Book Value of Equity</t>
+  </si>
+  <si>
+    <t>Book Value of Invested Capital</t>
+  </si>
+  <si>
+    <t>NOPAT</t>
+  </si>
+  <si>
+    <t>ROIC</t>
+  </si>
+  <si>
+    <t>Shareholder's Equity</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities &amp; Shareholder's Equity</t>
+  </si>
+  <si>
+    <t>CALC</t>
+  </si>
+  <si>
+    <t>OtherAccruedLiabilitiesCurrent</t>
+  </si>
+  <si>
+    <t>AvailableForSaleSecuritiesCurrent</t>
+  </si>
+  <si>
+    <t>Short Term Debt</t>
+  </si>
+  <si>
+    <t>CommercialPaper</t>
+  </si>
+  <si>
+    <t>LongTermDebtAndCapitalLeaseObligations</t>
+  </si>
+  <si>
+    <t>Long Term Debt</t>
+  </si>
+  <si>
+    <t>Accrued Expenses</t>
+  </si>
+  <si>
+    <t>LongTermDebtAndCapitalLeaseObligationsCurrent</t>
+  </si>
+  <si>
+    <t>Long Term Debt with CapLeaseObj</t>
+  </si>
+  <si>
+    <t>Invested Capital</t>
   </si>
 </sst>
 </file>
@@ -750,7 +804,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,12 +814,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,12 +836,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9E6FF3-6ECC-4982-8E9D-6D397E661C62}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,39 +1170,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>9</v>
@@ -1169,13 +1216,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>11</v>
@@ -1183,19 +1230,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>12</v>
@@ -1203,19 +1250,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>13</v>
@@ -1223,19 +1270,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>14</v>
@@ -1243,19 +1290,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <v>16</v>
@@ -1263,19 +1310,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8">
         <v>18</v>
@@ -1289,13 +1336,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>25</v>
@@ -1303,39 +1350,39 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>247</v>
       </c>
       <c r="B10">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="4">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="3">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>31</v>
@@ -1343,19 +1390,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="B12">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>22</v>
@@ -1363,423 +1410,697 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>246</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>245</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F14">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F15">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F16">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F17">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F18">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="1">
-        <v>3</v>
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="4">
-        <v>14</v>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="4">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
         <v>5</v>
       </c>
-      <c r="B22">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="1">
-        <v>7</v>
-      </c>
       <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
         <v>8</v>
       </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="1">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26">
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="1">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="1">
         <v>11</v>
       </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="3" t="str">
-        <f>A28</f>
-        <v>Tax rate assumption</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3">
-        <f>B28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29">
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>225</v>
-      </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>216</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>228</v>
       </c>
-      <c r="E32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>230</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>231</v>
       </c>
-      <c r="E34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C40" t="s">
+        <v>240</v>
+      </c>
+      <c r="F40">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>232</v>
       </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" t="s">
-        <v>55</v>
+      <c r="C41" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" t="s">
+        <v>240</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
+        <v>240</v>
+      </c>
+      <c r="F46">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>238</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" s="1">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>242</v>
+      </c>
+      <c r="E49" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>249</v>
+      </c>
+      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>248</v>
+      </c>
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>250</v>
+      </c>
+      <c r="C52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>250</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F28" xr:uid="{53754A5C-8C28-4DC2-B34B-DD0BCAD8CA1D}"/>
-  <sortState ref="G2:I30">
-    <sortCondition ref="I2:I30"/>
+  <autoFilter ref="A1:F30" xr:uid="{53754A5C-8C28-4DC2-B34B-DD0BCAD8CA1D}"/>
+  <sortState ref="G2:I32">
+    <sortCondition ref="I2:I32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1805,27 +2126,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>27</v>
@@ -1835,1076 +2156,1076 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C12">
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C21">
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F22" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F24" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C28">
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C29">
         <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C31">
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F31" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32">
         <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F32" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F33" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F34" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C36">
         <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C37">
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F37" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F38" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C39">
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C40">
         <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C41">
         <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C42">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C43">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F43" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C44">
         <v>29</v>
       </c>
       <c r="E44" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F44" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F45" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C46">
         <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F46" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C47">
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F47" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C49">
         <v>50</v>
       </c>
       <c r="E49" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F49" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C50">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F50" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C51">
         <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F51" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C52">
         <v>30</v>
       </c>
       <c r="E52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F53" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F54" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F55" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F56" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F57" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F58" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F59" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F60" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F61" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F62" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F63" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F64" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F65" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F66" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F67" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F69" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F70" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F71" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F72" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F73" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F74" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F76" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F77" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F78" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F79" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>